<commit_message>
3.0.14 sealed class is always final.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtSealedSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtSealedSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14632B8A-4AED-A24E-A6A2-723CFCFFE207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA149810-3B56-E042-9F64-F352D1493EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>クラス名</t>
   </si>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1786,9 +1786,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="59" t="s">
-        <v>31</v>
-      </c>
+      <c r="C17" s="59"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>

</xml_diff>